<commit_message>
APM Mobile seems functional (site still sketch)
</commit_message>
<xml_diff>
--- a/APMMOB/Test.xlsx
+++ b/APMMOB/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\PortTerminalScraping\TPJAX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\PortTerminalScraping\APMMOB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,208 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
-  <si>
-    <t>TLLU6021671</t>
-  </si>
-  <si>
-    <t>DIMITRA C</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829872</t>
-  </si>
-  <si>
-    <t>LCBV04707800</t>
-  </si>
-  <si>
-    <t>KKFU7847211</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829879</t>
-  </si>
-  <si>
-    <t>LCBV04721400</t>
-  </si>
-  <si>
-    <t>BSIU9695626</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829875</t>
-  </si>
-  <si>
-    <t>LCBV04718300</t>
-  </si>
-  <si>
-    <t>TCNU6880505</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829878</t>
-  </si>
-  <si>
-    <t>LCBV04708900</t>
-  </si>
-  <si>
-    <t>CXDU1242041</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829874</t>
-  </si>
-  <si>
-    <t>LCBV04719400</t>
-  </si>
-  <si>
-    <t>NYKU4817831</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829873</t>
-  </si>
-  <si>
-    <t>LCBV04720300</t>
-  </si>
-  <si>
-    <t>SEGU5810718</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829876</t>
-  </si>
-  <si>
-    <t>LCBV04716800</t>
-  </si>
-  <si>
-    <t>TLLU5443081</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829877</t>
-  </si>
-  <si>
-    <t>LCBV04709300</t>
-  </si>
-  <si>
-    <t>TCNU5156028</t>
-  </si>
-  <si>
-    <t>CHI1153604-CHI7829880</t>
-  </si>
-  <si>
-    <t>LCBV04706700</t>
-  </si>
-  <si>
-    <t>TLLU5691940</t>
-  </si>
-  <si>
-    <t>MOL MARVEL</t>
-  </si>
-  <si>
-    <t>CHI1153639-CHI7829991</t>
-  </si>
-  <si>
-    <t>TA8RF1832300</t>
-  </si>
-  <si>
-    <t>NYKU4813559</t>
-  </si>
-  <si>
-    <t>VIENNA EXPRESS</t>
-  </si>
-  <si>
-    <t>CHI1153644-CHI7829946</t>
-  </si>
-  <si>
-    <t>SH9FT8852800</t>
-  </si>
-  <si>
-    <t>TCLU1491294</t>
-  </si>
-  <si>
-    <t>MOL MAXIM</t>
-  </si>
-  <si>
-    <t>CHI1153645-CHI7829947</t>
-  </si>
-  <si>
-    <t>SH9FT8862900</t>
-  </si>
-  <si>
-    <t>CAXU8045406</t>
-  </si>
-  <si>
-    <t>CHICAGO EXPRESS</t>
-  </si>
-  <si>
-    <t>CHI1153649-CHI7829972</t>
-  </si>
-  <si>
-    <t>SZPV40171600</t>
-  </si>
-  <si>
-    <t>KKFU8119329</t>
-  </si>
-  <si>
-    <t>YM MOVEMENT</t>
-  </si>
-  <si>
-    <t>CHI1153652-CHI7829977</t>
-  </si>
-  <si>
-    <t>SGNV31086800</t>
-  </si>
-  <si>
-    <t>TRLU7628172</t>
-  </si>
-  <si>
-    <t>BRIGHTON</t>
-  </si>
-  <si>
-    <t>CHI1153651-CHI7829979</t>
-  </si>
-  <si>
-    <t>PNHV02844300</t>
-  </si>
-  <si>
-    <t>TCNU4411957</t>
-  </si>
-  <si>
-    <t>CHI1153650-CHI7829990</t>
-  </si>
-  <si>
-    <t>TA8DE2199400</t>
-  </si>
-  <si>
-    <t>TCNU4857445</t>
-  </si>
-  <si>
-    <t>CHI1153651-CHI7829980</t>
-  </si>
-  <si>
-    <t>PNHV02851800</t>
-  </si>
-  <si>
-    <t>TCNU4969722</t>
-  </si>
-  <si>
-    <t>CHI1153650-CHI7829989</t>
-  </si>
-  <si>
-    <t>TA8DE2200800</t>
-  </si>
-  <si>
-    <t>TEMU8723850</t>
-  </si>
-  <si>
-    <t>CHI1153652-CHI7829976</t>
-  </si>
-  <si>
-    <t>SGNV30205700</t>
-  </si>
-  <si>
-    <t>TGHU6209130</t>
-  </si>
-  <si>
-    <t>CHI1153652-CHI7829978</t>
-  </si>
-  <si>
-    <t>SGNV35850400</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>Equipment Number</t>
   </si>
@@ -243,6 +42,204 @@
   </si>
   <si>
     <t>BOLNumber</t>
+  </si>
+  <si>
+    <t>MEDU2268989</t>
+  </si>
+  <si>
+    <t>MSC VANESSA</t>
+  </si>
+  <si>
+    <t>FR912E</t>
+  </si>
+  <si>
+    <t>9077904952-01</t>
+  </si>
+  <si>
+    <t>MEDUS7410013</t>
+  </si>
+  <si>
+    <t>MEDU4674396</t>
+  </si>
+  <si>
+    <t>9077904953-01</t>
+  </si>
+  <si>
+    <t>MEDUS7410021</t>
+  </si>
+  <si>
+    <t>MSCU4878578</t>
+  </si>
+  <si>
+    <t>9077904954-01</t>
+  </si>
+  <si>
+    <t>MEDUS7488837</t>
+  </si>
+  <si>
+    <t>MSCU5531562</t>
+  </si>
+  <si>
+    <t>9077904955-01</t>
+  </si>
+  <si>
+    <t>MEDUS7472146</t>
+  </si>
+  <si>
+    <t>CPWU2925926</t>
+  </si>
+  <si>
+    <t>COSCO GENOA</t>
+  </si>
+  <si>
+    <t>041E</t>
+  </si>
+  <si>
+    <t>9078904109-01</t>
+  </si>
+  <si>
+    <t>COSU6199996500</t>
+  </si>
+  <si>
+    <t>TCNU7367858</t>
+  </si>
+  <si>
+    <t>CMA CGM LA SCALA</t>
+  </si>
+  <si>
+    <t>OPG3FE1MA</t>
+  </si>
+  <si>
+    <t>9071905863-01</t>
+  </si>
+  <si>
+    <t>EGLV156900065275</t>
+  </si>
+  <si>
+    <t>TEMU6135586</t>
+  </si>
+  <si>
+    <t>9071905864-01</t>
+  </si>
+  <si>
+    <t>TCNU6524227</t>
+  </si>
+  <si>
+    <t>9071905865-01</t>
+  </si>
+  <si>
+    <t>TCNU7359940</t>
+  </si>
+  <si>
+    <t>9071905866-01</t>
+  </si>
+  <si>
+    <t>TCNU6181154</t>
+  </si>
+  <si>
+    <t>9071905867-01</t>
+  </si>
+  <si>
+    <t>TCNU5214470</t>
+  </si>
+  <si>
+    <t>9071905868-01</t>
+  </si>
+  <si>
+    <t>MSCU4929253</t>
+  </si>
+  <si>
+    <t>MAERSK KALAMATA</t>
+  </si>
+  <si>
+    <t>913E</t>
+  </si>
+  <si>
+    <t>9072905108-01</t>
+  </si>
+  <si>
+    <t>MEDUS7472153</t>
+  </si>
+  <si>
+    <t>TRLU6600479</t>
+  </si>
+  <si>
+    <t>9072905102-01</t>
+  </si>
+  <si>
+    <t>MEDUS7551808</t>
+  </si>
+  <si>
+    <t>MSCU5972974</t>
+  </si>
+  <si>
+    <t>9072905110-01</t>
+  </si>
+  <si>
+    <t>MEDUQD538268</t>
+  </si>
+  <si>
+    <t>MSCU5881895</t>
+  </si>
+  <si>
+    <t>9072905111-01</t>
+  </si>
+  <si>
+    <t>MEDUQD538276</t>
+  </si>
+  <si>
+    <t>SEGU3049810</t>
+  </si>
+  <si>
+    <t>9078904316-01</t>
+  </si>
+  <si>
+    <t>COSU6203903980</t>
+  </si>
+  <si>
+    <t>OOLU0310488</t>
+  </si>
+  <si>
+    <t>NAVIOS UNITE</t>
+  </si>
+  <si>
+    <t>0PG3HE1MA</t>
+  </si>
+  <si>
+    <t>9072905903-01</t>
+  </si>
+  <si>
+    <t>COSU6194827780</t>
+  </si>
+  <si>
+    <t>EISU1871043</t>
+  </si>
+  <si>
+    <t>COSCO AUCKLAND</t>
+  </si>
+  <si>
+    <t>040E</t>
+  </si>
+  <si>
+    <t>9072905959-01</t>
+  </si>
+  <si>
+    <t>EGLV156900081670</t>
+  </si>
+  <si>
+    <t>TGHU6091474</t>
+  </si>
+  <si>
+    <t>9073905364-01</t>
+  </si>
+  <si>
+    <t>MEDUVN692227</t>
+  </si>
+  <si>
+    <t>MEDU8777324</t>
+  </si>
+  <si>
+    <t>9073905365-01</t>
   </si>
 </sst>
 </file>
@@ -563,369 +560,369 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A2" sqref="A2:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>304</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>304</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>304</v>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>304</v>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>304</v>
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>304</v>
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>304</v>
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>304</v>
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>304</v>
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
         <v>29</v>
-      </c>
-      <c r="C11">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12">
-        <v>59</v>
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
         <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="C14">
-        <v>81</v>
+      <c r="C14" t="s">
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16">
-        <v>103</v>
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19">
-        <v>46</v>
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>